<commit_message>
Re-wrote code specifically for Seed 6
Seed 6 never completes transition so the computations here are only valid for this particular seed.
</commit_message>
<xml_diff>
--- a/Thrust Resulsts Summary.xlsx
+++ b/Thrust Resulsts Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shash\Documents\GitHub\samaraAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDF7DC5-A24B-44BA-B76F-225DD13F401B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC42B287-BF65-4B56-82DA-48D18DE40246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{43FC6C5E-84DC-4039-A0CF-54CA44F837D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43FC6C5E-84DC-4039-A0CF-54CA44F837D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Seed</t>
   </si>
@@ -120,13 +120,57 @@
   </si>
   <si>
     <t>Chord [mm]</t>
+  </si>
+  <si>
+    <t>Omega: ω [RPS]</t>
+  </si>
+  <si>
+    <t>Omega: ω [RPM]</t>
+  </si>
+  <si>
+    <t>Average Thrust [N]</t>
+  </si>
+  <si>
+    <t>xNorm = x Position Normalized</t>
+  </si>
+  <si>
+    <t>Area [m^2]</t>
+  </si>
+  <si>
+    <t>Evaluation over last 10 time stamps</t>
+  </si>
+  <si>
+    <t>Last τ seconds over which values were extracted</t>
+  </si>
+  <si>
+    <t>Mass [kg]</t>
+  </si>
+  <si>
+    <r>
+      <t>Note, for Seed 6, the period of rotation was computed by taking the negative peak (around 0.5) and subtracting the positive peak. To get the period, this difference was multiplied by 2. It should be noted that this seed actually never reaches steady state so the results do not mean much.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (See Thrust Coeff)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,16 +178,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -151,18 +231,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -173,6 +407,219 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>580549</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219888B3-FB49-5CD0-2F67-53EC1AE51CEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3810000"/>
+          <a:ext cx="3809524" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>685315</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>37769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07EFCE8C-79CD-38BE-AC93-76831EBE8573}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="3714750"/>
+          <a:ext cx="3876190" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1161581</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>113969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47F0DC34-0B7A-C7B1-964F-BD3F293BB066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4686300" y="3790950"/>
+          <a:ext cx="3752381" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>380521</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8025045-ACD0-5B9B-D8B6-9A4C3A2D9C4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12563475" y="3724275"/>
+          <a:ext cx="3828571" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AACF6A9-68F5-4C09-96DB-64258EC9551E}" name="Table1" displayName="Table1" ref="B2:P6" totalsRowShown="0">
+  <autoFilter ref="B2:P6" xr:uid="{3AACF6A9-68F5-4C09-96DB-64258EC9551E}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{076489D6-3D2D-459B-A922-B452DE6C8382}" name="Seed"/>
+    <tableColumn id="2" xr3:uid="{23048464-97CD-46F1-B337-0BE6C36EA5D9}" name="Mass [g]"/>
+    <tableColumn id="15" xr3:uid="{ADC25D2B-C2E1-47A2-8537-281A6AB44FEF}" name="Mass [kg]" dataDxfId="0">
+      <calculatedColumnFormula>C3*0.001</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{9CF5C7A6-0FA1-49E0-A429-F8816CA66315}" name="Area [mm^2]"/>
+    <tableColumn id="14" xr3:uid="{4D64692F-8BFF-41F6-8F36-E6EF56841CEC}" name="Area [m^2]" dataDxfId="1">
+      <calculatedColumnFormula>Table1[[#This Row],[Area '[mm^2']]]*0.000001</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{842B4472-EE29-4A00-B9C2-A134BA371483}" name="Loading"/>
+    <tableColumn id="5" xr3:uid="{29E2F226-FF05-4B10-94D7-6E86BC3F231C}" name="Span [mm]"/>
+    <tableColumn id="6" xr3:uid="{73B3022C-5EA2-49FF-8587-D22321CE1CCB}" name="Chord [mm]"/>
+    <tableColumn id="7" xr3:uid="{4164DAA3-7F92-4CC1-9870-AD33C88CD474}" name="Aspect"/>
+    <tableColumn id="8" xr3:uid="{45C85D76-8400-4BF9-AB6B-ECF0B3405A2D}" name="Number of Evaluations">
+      <calculatedColumnFormula>10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{E0674460-ADDD-4798-9B20-636135D714F0}" name="Evaluation Duration [s]"/>
+    <tableColumn id="10" xr3:uid="{240F192D-90F2-4846-8210-CFF3FC6B5D63}" name="Omega: ω [RPS]"/>
+    <tableColumn id="11" xr3:uid="{8EF2048A-5850-48BE-B0BE-A54F8D48DC19}" name="Omega: ω [RPM]">
+      <calculatedColumnFormula>M3*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{8D200E75-A8BD-414C-889B-980C18942F58}" name="Average Thrust [N]"/>
+    <tableColumn id="13" xr3:uid="{5D0D6066-DEB9-4E45-A634-A51FBD817639}" name="Average Thrust Coefficient"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,20 +939,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DD9009-B34A-49C6-9CD4-28FFAF0FFF18}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -513,145 +976,293 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
         <v>0.4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">C3*0.001</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1">
+        <f>Table1[[#This Row],[Area '[mm^2']]]*0.000001</f>
+        <v>1.1687016962908798E-3</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>47.0639380678127</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <f>10</f>
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>1.00384368994235E-2</v>
-      </c>
-      <c r="K3">
+      <c r="L3">
+        <v>1.0025591810620601E-2</v>
+      </c>
+      <c r="M3">
+        <v>79.176173635061602</v>
+      </c>
+      <c r="N3">
+        <f>M3*60</f>
+        <v>4750.5704181036963</v>
+      </c>
+      <c r="O3">
+        <v>2.9501607254050701E-3</v>
+      </c>
+      <c r="P3">
         <v>8.74825940511266E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1">
+        <f>Table1[[#This Row],[Area '[mm^2']]]*0.000001</f>
+        <v>1.5222761139517798E-3</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f>10</f>
         <v>10</v>
       </c>
+      <c r="L4">
+        <v>1.0155502398325401E-2</v>
+      </c>
+      <c r="M4">
+        <v>16.338845970000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N6" si="1">M4*60</f>
+        <v>980.3307582000001</v>
+      </c>
+      <c r="O4">
+        <v>5.5860116901800504E-3</v>
+      </c>
+      <c r="P4">
+        <v>0.180705312011784</v>
+      </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5">
         <v>0.5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1">
+        <f>Table1[[#This Row],[Area '[mm^2']]]*0.000001</f>
+        <v>1.0501453453453399E-3</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f>10</f>
         <v>10</v>
       </c>
+      <c r="L5">
+        <v>0.01</v>
+      </c>
+      <c r="M5">
+        <v>111.328283649867</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>6679.6970189920203</v>
+      </c>
+      <c r="O5">
+        <v>3.8937229967331102E-3</v>
+      </c>
+      <c r="P5">
+        <v>5.5359926907532801E-3</v>
+      </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>47</v>
       </c>
       <c r="C6">
         <v>0.6</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1">
+        <f>Table1[[#This Row],[Area '[mm^2']]]*0.000001</f>
+        <v>9.4111958444931395E-4</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>45.032438890873699</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <f>10</f>
         <v>10</v>
       </c>
+      <c r="L6">
+        <v>1.1190738699007699E-2</v>
+      </c>
+      <c r="M6">
+        <v>55.503570019733303</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>3330.2142011839983</v>
+      </c>
+      <c r="O6">
+        <v>4.6841549052324596E-3</v>
+      </c>
+      <c r="P6">
+        <v>3.2341267204638903E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B10:K11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>